<commit_message>
added files on 22/10/2020
</commit_message>
<xml_diff>
--- a/resources/configFile/TestData.xlsx
+++ b/resources/configFile/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -27,31 +27,16 @@
     <t>password</t>
   </si>
   <si>
-    <t>mngr283898</t>
-  </si>
-  <si>
-    <t>gUdudUb</t>
-  </si>
-  <si>
     <t>runMode</t>
   </si>
   <si>
     <t>y</t>
   </si>
   <si>
-    <t>sumit</t>
-  </si>
-  <si>
-    <t>intel@01</t>
-  </si>
-  <si>
-    <t>sam</t>
-  </si>
-  <si>
-    <t>test@01</t>
-  </si>
-  <si>
-    <t>n</t>
+    <t>mngr289535</t>
+  </si>
+  <si>
+    <t>AtUpypU</t>
   </si>
 </sst>
 </file>
@@ -396,7 +381,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -407,7 +392,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -425,59 +410,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="B5" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>